<commit_message>
Update Remarks col for Calls & Messages, create leads. Provide new format and input fields and excel upload for required format of remarks
</commit_message>
<xml_diff>
--- a/app/Rules/calls.xlsx
+++ b/app/Rules/calls.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\mileleapp\mileleapp\storage\app\public\sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://milelemotors-my.sharepoint.com/personal/hammad_mukhtar_milele_com/Documents/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B424F69-4466-46DD-9748-A7040E09CBEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{6B424F69-4466-46DD-9748-A7040E09CBEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C46E95E-55D3-4286-AF19-6CC11306AC81}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{4663B284-774D-4BCD-932C-AC5EAC6AD582}"/>
+    <workbookView xWindow="6960" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{4663B284-774D-4BCD-932C-AC5EAC6AD582}"/>
   </bookViews>
   <sheets>
     <sheet name="LEAD_DATA" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8333" uniqueCount="8318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8344" uniqueCount="8329">
   <si>
     <t>CUSTOMER_NAME</t>
   </si>
@@ -24994,6 +24994,39 @@
   </si>
   <si>
     <t>low</t>
+  </si>
+  <si>
+    <t>CAR INTERESTED IN</t>
+  </si>
+  <si>
+    <t>PURPOSE OF PURCHASE</t>
+  </si>
+  <si>
+    <t>END USER</t>
+  </si>
+  <si>
+    <t>DESTINATION COUNTRY</t>
+  </si>
+  <si>
+    <t>PLANNED UNITS</t>
+  </si>
+  <si>
+    <t>EXPERIENCE WITH UAE SOURCING</t>
+  </si>
+  <si>
+    <t>SHIPPING ASSISTANCE REQUIRED</t>
+  </si>
+  <si>
+    <t>PAYMENT METHOD</t>
+  </si>
+  <si>
+    <t>PREVIOUS PURCHASE HISTORY</t>
+  </si>
+  <si>
+    <t>PURCHASE TIMELINE</t>
+  </si>
+  <si>
+    <t>ADDITIONAL NOTES</t>
   </si>
 </sst>
 </file>
@@ -25554,10 +25587,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35898B72-8369-41D4-A188-7FA8EB09E0FB}">
-  <dimension ref="A1:H7862"/>
+  <dimension ref="A1:S7862"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -25570,9 +25603,20 @@
     <col min="6" max="6" width="54.59765625" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="11.06640625" customWidth="1"/>
+    <col min="9" max="9" width="16.86328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.86328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.53125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="28.73046875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.1328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.46484375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.06640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -25597,8 +25641,41 @@
       <c r="H1" s="1" t="s">
         <v>8314</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I1" s="1" t="s">
+        <v>8318</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8319</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8320</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>8321</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>8322</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>8323</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>8324</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>8325</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>8326</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>8327</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>8328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -25621,7 +25698,7 @@
         <v>8315</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -25644,7 +25721,7 @@
         <v>8316</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -25667,7 +25744,7 @@
         <v>8317</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -25687,7 +25764,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -25707,7 +25784,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -25727,7 +25804,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -25747,7 +25824,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -25767,7 +25844,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>68</v>
       </c>
@@ -25787,7 +25864,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>74</v>
       </c>
@@ -25807,7 +25884,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>80</v>
       </c>
@@ -25827,7 +25904,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>8304</v>
       </c>
@@ -25847,7 +25924,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
         <v>86</v>
       </c>
@@ -25864,7 +25941,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>91</v>
       </c>
@@ -25881,7 +25958,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
         <v>96</v>
       </c>
@@ -66530,15 +66607,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -66572,6 +66640,15 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D8457CE-DE03-474A-A3EE-2E283389F184}">
   <ds:schemaRefs>
@@ -66593,14 +66670,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61120D28-EB26-4BEE-B363-F609F3FF3AF1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BA1EF99-9058-4FC1-B716-D565CB90A035}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -66612,6 +66681,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61120D28-EB26-4BEE-B363-F609F3FF3AF1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{fd7d97ec-46e1-4519-ab4e-0e4708b9a3cf}" enabled="0" method="" siteId="{fd7d97ec-46e1-4519-ab4e-0e4708b9a3cf}" removed="1"/>

</xml_diff>